<commit_message>
edited kws and blog in prototyp
</commit_message>
<xml_diff>
--- a/kws/kws-priradene.xlsx
+++ b/kws/kws-priradene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matusrebros/super/kws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF105C70-FB2F-8441-B10A-0145F2CC16A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C23F84-5A65-3144-B213-17B40412A261}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1460" windowWidth="28040" windowHeight="17440" xr2:uid="{24AB14E7-762D-AE4E-B4A7-B13D6B471532}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="369">
   <si>
     <t>#</t>
   </si>
@@ -1129,6 +1129,9 @@
   </si>
   <si>
     <t>webová analytika</t>
+  </si>
+  <si>
+    <t>pridať do sekcie TVORBA WEB STRÁNOK</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1240,127 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="200">
+  <dxfs count="215">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2614,202 +2737,202 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E1CF4BF-75F8-9140-B94C-5EB0541D09F5}" name="Table1" displayName="Table1" ref="A2:F14" totalsRowShown="0" dataDxfId="199">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E1CF4BF-75F8-9140-B94C-5EB0541D09F5}" name="Table1" displayName="Table1" ref="A2:F14" totalsRowShown="0" dataDxfId="214">
   <autoFilter ref="A2:F14" xr:uid="{74E50701-1A0A-894E-9143-9FEFF3FB7E7D}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7E2F558B-F58E-0C4D-BB56-5AA65B95B592}" name="#"/>
     <tableColumn id="2" xr3:uid="{4627E11D-6659-0946-969B-79A6AEF6B3C9}" name="KW"/>
-    <tableColumn id="3" xr3:uid="{C23F3803-D413-0B4B-B9FA-FE2BB29F06E6}" name="VOLUME" dataDxfId="198"/>
-    <tableColumn id="4" xr3:uid="{B58DF622-F89E-8941-B0FC-583C368F9B99}" name="CPC" dataDxfId="197"/>
-    <tableColumn id="5" xr3:uid="{886F3236-A825-CE4D-9DDB-013936859674}" name="PD" dataDxfId="196"/>
-    <tableColumn id="6" xr3:uid="{5198577F-51C6-9246-8B59-7EF18AE961D7}" name="SD" dataDxfId="195"/>
+    <tableColumn id="3" xr3:uid="{C23F3803-D413-0B4B-B9FA-FE2BB29F06E6}" name="VOLUME" dataDxfId="213"/>
+    <tableColumn id="4" xr3:uid="{B58DF622-F89E-8941-B0FC-583C368F9B99}" name="CPC" dataDxfId="212"/>
+    <tableColumn id="5" xr3:uid="{886F3236-A825-CE4D-9DDB-013936859674}" name="PD" dataDxfId="211"/>
+    <tableColumn id="6" xr3:uid="{5198577F-51C6-9246-8B59-7EF18AE961D7}" name="SD" dataDxfId="210"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E7A93C3E-0A6E-9547-B6AC-70F5053DA86D}" name="Table10" displayName="Table10" ref="A99:F103" totalsRowShown="0" headerRowDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E7A93C3E-0A6E-9547-B6AC-70F5053DA86D}" name="Table10" displayName="Table10" ref="A99:F103" totalsRowShown="0" headerRowDxfId="178">
   <autoFilter ref="A99:F103" xr:uid="{E7E42209-AA07-9B40-B6FB-8962E55B2429}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E61304BA-FD70-7B4A-8F8F-2353A025E3E0}" name="#"/>
-    <tableColumn id="2" xr3:uid="{26DE8984-F2E3-2D45-A01C-DC4E4BFCE41E}" name="KW" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{F032AA5E-BBEA-0F4D-A120-66BB691369E0}" name="VOLUME" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{1F751F65-1511-014F-93F8-FAF144C07979}" name="CPC" dataDxfId="82"/>
-    <tableColumn id="5" xr3:uid="{74A13CC7-DD15-F54C-B7A4-E7AB3E4E9E2D}" name="PD" dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{A6B5B915-D592-D44D-A3F7-93AF5CF101F3}" name="SD" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{26DE8984-F2E3-2D45-A01C-DC4E4BFCE41E}" name="KW" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{F032AA5E-BBEA-0F4D-A120-66BB691369E0}" name="VOLUME" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{1F751F65-1511-014F-93F8-FAF144C07979}" name="CPC" dataDxfId="97"/>
+    <tableColumn id="5" xr3:uid="{74A13CC7-DD15-F54C-B7A4-E7AB3E4E9E2D}" name="PD" dataDxfId="96"/>
+    <tableColumn id="6" xr3:uid="{A6B5B915-D592-D44D-A3F7-93AF5CF101F3}" name="SD" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8E8E6AE0-16A0-4D47-901E-E2E6BFD9409A}" name="Table11" displayName="Table11" ref="A107:F109" totalsRowShown="0" headerRowDxfId="162">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8E8E6AE0-16A0-4D47-901E-E2E6BFD9409A}" name="Table11" displayName="Table11" ref="A107:F109" totalsRowShown="0" headerRowDxfId="177">
   <autoFilter ref="A107:F109" xr:uid="{4305766E-D3AF-6441-ABB3-69758F113174}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A6788509-2311-1146-8FFA-EF930A8EA465}" name="#"/>
-    <tableColumn id="2" xr3:uid="{ED20E06E-FCF5-644F-90BB-58B5133565AF}" name="KW" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{18E36775-FB96-CA49-9F91-2DA953D7DB35}" name="VOLUME" dataDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{6CCE875C-4F2A-8A4B-9BF7-EDECB81E9155}" name="CPC" dataDxfId="87"/>
-    <tableColumn id="5" xr3:uid="{CDCADAC3-AE5F-7C42-8849-43DF27FEA349}" name="PD" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{E76A6225-F40D-5E45-A05D-30DF3A9ADF7D}" name="SD" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{ED20E06E-FCF5-644F-90BB-58B5133565AF}" name="KW" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{18E36775-FB96-CA49-9F91-2DA953D7DB35}" name="VOLUME" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{6CCE875C-4F2A-8A4B-9BF7-EDECB81E9155}" name="CPC" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{CDCADAC3-AE5F-7C42-8849-43DF27FEA349}" name="PD" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{E76A6225-F40D-5E45-A05D-30DF3A9ADF7D}" name="SD" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{1CAF062D-CFD8-C54C-ADD5-C31993589BBC}" name="Table12" displayName="Table12" ref="A112:F114" totalsRowShown="0" headerRowDxfId="161">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{1CAF062D-CFD8-C54C-ADD5-C31993589BBC}" name="Table12" displayName="Table12" ref="A112:F114" totalsRowShown="0" headerRowDxfId="176">
   <autoFilter ref="A112:F114" xr:uid="{002C4BF5-9DCC-4542-B22C-088766D48D54}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{14DFE193-5DF2-7B46-8D37-E4B852686543}" name="#"/>
-    <tableColumn id="2" xr3:uid="{22120B33-C216-C849-8733-271D62D42637}" name="KW" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{28D313CE-9A65-9C4C-B37F-26FD2CB8F220}" name="VOLUME" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{9FD75F01-6BEE-6740-8E60-27D73CC2C6C6}" name="CPC" dataDxfId="92"/>
-    <tableColumn id="5" xr3:uid="{D3C31E8C-6969-9D48-877D-66630FE990C7}" name="PD" dataDxfId="91"/>
-    <tableColumn id="6" xr3:uid="{485A3899-A8D1-9C47-AED5-54F7AB5FB17D}" name="SD" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{22120B33-C216-C849-8733-271D62D42637}" name="KW" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{28D313CE-9A65-9C4C-B37F-26FD2CB8F220}" name="VOLUME" dataDxfId="108"/>
+    <tableColumn id="4" xr3:uid="{9FD75F01-6BEE-6740-8E60-27D73CC2C6C6}" name="CPC" dataDxfId="107"/>
+    <tableColumn id="5" xr3:uid="{D3C31E8C-6969-9D48-877D-66630FE990C7}" name="PD" dataDxfId="106"/>
+    <tableColumn id="6" xr3:uid="{485A3899-A8D1-9C47-AED5-54F7AB5FB17D}" name="SD" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3288C749-29DB-C248-A15B-C2D6C80E411A}" name="Table13" displayName="Table13" ref="A118:F119" totalsRowShown="0" headerRowDxfId="160">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3288C749-29DB-C248-A15B-C2D6C80E411A}" name="Table13" displayName="Table13" ref="A118:F119" totalsRowShown="0" headerRowDxfId="175">
   <autoFilter ref="A118:F119" xr:uid="{68793F86-3D24-0F4A-990D-C7CF9E15EEEE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C083CA5A-CED1-2544-A924-BF8EEF828141}" name="#"/>
-    <tableColumn id="2" xr3:uid="{DDDCE6E4-079D-8F44-BEDC-2D8E1D809960}" name="KW" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{DF554EFA-9A03-8044-8EA2-F767F7889644}" name="VOLUME" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{41663514-B724-344B-B562-C6FC56BB1299}" name="CPC" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{EC53C1B7-E67E-1B41-AF37-C8CD92815570}" name="PD" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{C6B41853-1E9B-8447-B340-4AC432D537BB}" name="SD" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{DDDCE6E4-079D-8F44-BEDC-2D8E1D809960}" name="KW" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{DF554EFA-9A03-8044-8EA2-F767F7889644}" name="VOLUME" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{41663514-B724-344B-B562-C6FC56BB1299}" name="CPC" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{EC53C1B7-E67E-1B41-AF37-C8CD92815570}" name="PD" dataDxfId="91"/>
+    <tableColumn id="6" xr3:uid="{C6B41853-1E9B-8447-B340-4AC432D537BB}" name="SD" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{EB25DF35-48A6-8E41-AF07-9C9F53F94A24}" name="Table14" displayName="Table14" ref="A124:F127" totalsRowShown="0" headerRowDxfId="159">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{EB25DF35-48A6-8E41-AF07-9C9F53F94A24}" name="Table14" displayName="Table14" ref="A124:F127" totalsRowShown="0" headerRowDxfId="174">
   <autoFilter ref="A124:F127" xr:uid="{07B063AC-5CC6-6F49-98B4-7F9FF1957CE3}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3BA58D70-94CD-EF48-B010-983DDE9975B7}" name="#"/>
-    <tableColumn id="2" xr3:uid="{FC742E95-A6F7-D44B-8AAC-836BB2862645}" name="KW" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{2A66C610-D5BD-994A-9D38-C95667CC3C2F}" name="VOLUME" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{6473FBC7-D46E-B941-80F5-CACAB22AAF43}" name="CPC" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{73211850-4DBC-6343-A290-B22C77613CB4}" name="PD" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{895FF0DC-6096-7F48-B707-30E1C37B975B}" name="SD" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{FC742E95-A6F7-D44B-8AAC-836BB2862645}" name="KW" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{2A66C610-D5BD-994A-9D38-C95667CC3C2F}" name="VOLUME" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{6473FBC7-D46E-B941-80F5-CACAB22AAF43}" name="CPC" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{73211850-4DBC-6343-A290-B22C77613CB4}" name="PD" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{895FF0DC-6096-7F48-B707-30E1C37B975B}" name="SD" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0E301EB3-0244-BD4E-BE42-7E383DC067A8}" name="Table15" displayName="Table15" ref="A130:F131" totalsRowShown="0" headerRowDxfId="158">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{0E301EB3-0244-BD4E-BE42-7E383DC067A8}" name="Table15" displayName="Table15" ref="A130:F131" totalsRowShown="0" headerRowDxfId="173">
   <autoFilter ref="A130:F131" xr:uid="{7305680E-492B-6D41-8A11-2ADF96E886A6}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2B20E6D4-326E-7B47-88A6-D7848863753C}" name="#"/>
-    <tableColumn id="2" xr3:uid="{177402D9-0A07-F84F-81D9-540BC822D7F5}" name="KW" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{AE3795E6-7C5C-FC44-92CB-D77E97FE8F39}" name="VOLUME" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{DA1180F6-110E-8043-BE9C-9278D70F8A5F}" name="CPC" dataDxfId="107"/>
-    <tableColumn id="5" xr3:uid="{834E0BB8-A662-2340-8C26-906F358988FD}" name="PD" dataDxfId="106"/>
-    <tableColumn id="6" xr3:uid="{3EEF1959-AB35-2C49-B514-927AA19198F9}" name="SD" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{177402D9-0A07-F84F-81D9-540BC822D7F5}" name="KW" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{AE3795E6-7C5C-FC44-92CB-D77E97FE8F39}" name="VOLUME" dataDxfId="123"/>
+    <tableColumn id="4" xr3:uid="{DA1180F6-110E-8043-BE9C-9278D70F8A5F}" name="CPC" dataDxfId="122"/>
+    <tableColumn id="5" xr3:uid="{834E0BB8-A662-2340-8C26-906F358988FD}" name="PD" dataDxfId="121"/>
+    <tableColumn id="6" xr3:uid="{3EEF1959-AB35-2C49-B514-927AA19198F9}" name="SD" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F69D9181-DC29-FC42-A5AD-77A71835AC1B}" name="Table16" displayName="Table16" ref="A134:F135" totalsRowShown="0" headerRowDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F69D9181-DC29-FC42-A5AD-77A71835AC1B}" name="Table16" displayName="Table16" ref="A134:F135" totalsRowShown="0" headerRowDxfId="172">
   <autoFilter ref="A134:F135" xr:uid="{A62F0686-D32F-5A4D-868A-DA1259E3D6B5}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{F4FEA10C-19CD-BC4A-A256-125D4FDAF276}" name="#"/>
-    <tableColumn id="2" xr3:uid="{CF5ABF10-84A7-8A4B-877E-F37F73BAD95A}" name="KW" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{CFCEB75F-27D4-A241-B5F5-B1ABD9E41043}" name="VOLUME" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{516B962D-2935-9844-B203-5E5153227BE0}" name="CPC" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{2E9BE74C-9971-9F44-A8C7-A3D8745FF59E}" name="PD" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{E270E56B-2248-6E45-9837-92FA5FE80197}" name="SD" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{CF5ABF10-84A7-8A4B-877E-F37F73BAD95A}" name="KW" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{CFCEB75F-27D4-A241-B5F5-B1ABD9E41043}" name="VOLUME" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{516B962D-2935-9844-B203-5E5153227BE0}" name="CPC" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{2E9BE74C-9971-9F44-A8C7-A3D8745FF59E}" name="PD" dataDxfId="81"/>
+    <tableColumn id="6" xr3:uid="{E270E56B-2248-6E45-9837-92FA5FE80197}" name="SD" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{CCED5B12-FED4-604A-B637-36938155EAB1}" name="Table17" displayName="Table17" ref="A138:F139" totalsRowShown="0" headerRowDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{CCED5B12-FED4-604A-B637-36938155EAB1}" name="Table17" displayName="Table17" ref="A138:F139" totalsRowShown="0" headerRowDxfId="171">
   <autoFilter ref="A138:F139" xr:uid="{7EE444A1-7AE5-A54E-8997-15CC36FA126B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4CF1A1F9-8026-0543-82EF-3F3CA64F1353}" name="#"/>
-    <tableColumn id="2" xr3:uid="{7B2FBCF4-8EC0-0F46-A8DE-28A6BCC1FE19}" name="KW" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{88F7B4C4-6673-2243-A584-8D737DFC48C6}" name="VOLUME" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{89CC3E3A-4522-FB48-88DA-FB8C58CA5E3F}" name="CPC" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{0599F371-B9EB-784E-B7DB-94D246E76605}" name="PD" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{DC38DE6B-9F84-724B-85A4-B7FF531168EF}" name="SD" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{7B2FBCF4-8EC0-0F46-A8DE-28A6BCC1FE19}" name="KW" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{88F7B4C4-6673-2243-A584-8D737DFC48C6}" name="VOLUME" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{89CC3E3A-4522-FB48-88DA-FB8C58CA5E3F}" name="CPC" dataDxfId="87"/>
+    <tableColumn id="5" xr3:uid="{0599F371-B9EB-784E-B7DB-94D246E76605}" name="PD" dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{DC38DE6B-9F84-724B-85A4-B7FF531168EF}" name="SD" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{E4880F1C-B94D-D74B-9915-22097FC6285F}" name="Table18" displayName="Table18" ref="A143:F144" totalsRowShown="0" headerRowDxfId="155">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{E4880F1C-B94D-D74B-9915-22097FC6285F}" name="Table18" displayName="Table18" ref="A143:F144" totalsRowShown="0" headerRowDxfId="170">
   <autoFilter ref="A143:F144" xr:uid="{E6DE82C3-2D0B-4F4D-8F39-D1DA689D19CB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B662F13E-B492-214B-8931-01BDCEDCC41E}" name="#"/>
-    <tableColumn id="2" xr3:uid="{57C44F1E-A8BB-3F4E-8DAE-52F8B56261D9}" name="KW" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{B091047A-9F2F-3541-BADA-AD774EBE5331}" name="VOLUME" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{12FA177C-FBC7-C640-8B48-C4B014FB6A20}" name="CPC" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{7411FCA2-7CE8-C140-947E-6B7E54883872}" name="PD" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{DD369330-2665-6340-9421-371896A214BF}" name="SD" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{57C44F1E-A8BB-3F4E-8DAE-52F8B56261D9}" name="KW" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{B091047A-9F2F-3541-BADA-AD774EBE5331}" name="VOLUME" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{12FA177C-FBC7-C640-8B48-C4B014FB6A20}" name="CPC" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{7411FCA2-7CE8-C140-947E-6B7E54883872}" name="PD" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{DD369330-2665-6340-9421-371896A214BF}" name="SD" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{4C564B1B-0DD7-D347-A188-900BB14F90A1}" name="Table19" displayName="Table19" ref="A147:F148" totalsRowShown="0" headerRowDxfId="154">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{4C564B1B-0DD7-D347-A188-900BB14F90A1}" name="Table19" displayName="Table19" ref="A147:F148" totalsRowShown="0" headerRowDxfId="169">
   <autoFilter ref="A147:F148" xr:uid="{82E2DF75-CE68-2049-A332-A8A898978DEB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2EE0FD00-9808-A048-A1D7-26DF234957CF}" name="#"/>
-    <tableColumn id="2" xr3:uid="{01B5B0A8-4981-7549-9823-F4C5C67D5D1D}" name="KW"/>
-    <tableColumn id="3" xr3:uid="{58CA2B5C-D66A-4A48-86CB-8497241B2329}" name="VOLUME"/>
-    <tableColumn id="4" xr3:uid="{99EB0716-F95B-924D-B3F3-76D44C0A85AD}" name="CPC"/>
-    <tableColumn id="5" xr3:uid="{76343CE1-EE62-1C41-A722-91AAA774A974}" name="PD"/>
-    <tableColumn id="6" xr3:uid="{BB2E850E-B030-5E4E-BE4C-F8B8591EBC6F}" name="SD"/>
+    <tableColumn id="2" xr3:uid="{01B5B0A8-4981-7549-9823-F4C5C67D5D1D}" name="KW" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{58CA2B5C-D66A-4A48-86CB-8497241B2329}" name="VOLUME" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{99EB0716-F95B-924D-B3F3-76D44C0A85AD}" name="CPC" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{76343CE1-EE62-1C41-A722-91AAA774A974}" name="PD" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{BB2E850E-B030-5E4E-BE4C-F8B8591EBC6F}" name="SD" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D48F073F-2499-0248-B6F9-6DCD366691D7}" name="Table2" displayName="Table2" ref="A20:F28" totalsRowShown="0" headerRowDxfId="193" dataDxfId="194">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D48F073F-2499-0248-B6F9-6DCD366691D7}" name="Table2" displayName="Table2" ref="A20:F28" totalsRowShown="0" headerRowDxfId="208" dataDxfId="209">
   <autoFilter ref="A20:F28" xr:uid="{2A107C8F-0360-1140-9931-4B2DFB244DB4}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{132A3B5B-67A2-6F4C-9B7C-68E1557A365C}" name="#"/>
-    <tableColumn id="2" xr3:uid="{F9827C56-5234-A445-8857-7911661EBCA4}" name="KW" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{EEC35316-54F0-924C-882C-651D0C826C70}" name="VOLUME" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{F6EA3307-AF1D-754B-85D2-A00BB081CB66}" name="CPC" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{25251231-2500-B24D-9F4D-92B0EDCB914B}" name="PD" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{A081A408-F986-3A44-81B9-B87E91DB643C}" name="SD" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{F9827C56-5234-A445-8857-7911661EBCA4}" name="KW" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{EEC35316-54F0-924C-882C-651D0C826C70}" name="VOLUME" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{F6EA3307-AF1D-754B-85D2-A00BB081CB66}" name="CPC" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{25251231-2500-B24D-9F4D-92B0EDCB914B}" name="PD" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{A081A408-F986-3A44-81B9-B87E91DB643C}" name="SD" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{AE8F46DB-ECF7-1546-80E0-03AB32B24A7F}" name="Table20" displayName="Table20" ref="A152:F153" totalsRowShown="0" headerRowDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{AE8F46DB-ECF7-1546-80E0-03AB32B24A7F}" name="Table20" displayName="Table20" ref="A152:F153" totalsRowShown="0" headerRowDxfId="168">
   <autoFilter ref="A152:F153" xr:uid="{F2B18E16-58EF-5D41-8091-EF95A67FD6D4}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{F0A66B5C-E51A-064B-8CD8-7953EF424F1D}" name="#"/>
-    <tableColumn id="2" xr3:uid="{67E0028D-9048-A946-85E9-9C0E237208C7}" name="KW" dataDxfId="114"/>
-    <tableColumn id="3" xr3:uid="{626E579B-E951-9646-8C5F-693F94A026AF}" name="VOLUME" dataDxfId="113"/>
-    <tableColumn id="4" xr3:uid="{C79CF989-127A-CE4A-A7A5-FD447EECFD8F}" name="CPC" dataDxfId="112"/>
-    <tableColumn id="5" xr3:uid="{B3D4E7E5-3492-4247-8FB1-608779BBE7A5}" name="PD" dataDxfId="111"/>
-    <tableColumn id="6" xr3:uid="{1140D62C-01F3-1F4A-84BA-7E074556E233}" name="SD" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{67E0028D-9048-A946-85E9-9C0E237208C7}" name="KW" dataDxfId="129"/>
+    <tableColumn id="3" xr3:uid="{626E579B-E951-9646-8C5F-693F94A026AF}" name="VOLUME" dataDxfId="128"/>
+    <tableColumn id="4" xr3:uid="{C79CF989-127A-CE4A-A7A5-FD447EECFD8F}" name="CPC" dataDxfId="127"/>
+    <tableColumn id="5" xr3:uid="{B3D4E7E5-3492-4247-8FB1-608779BBE7A5}" name="PD" dataDxfId="126"/>
+    <tableColumn id="6" xr3:uid="{1140D62C-01F3-1F4A-84BA-7E074556E233}" name="SD" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{72195EDD-4C36-8D43-A297-8A3055ABC67C}" name="Table21" displayName="Table21" ref="A157:F160" totalsRowShown="0" headerRowDxfId="152">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{72195EDD-4C36-8D43-A297-8A3055ABC67C}" name="Table21" displayName="Table21" ref="A157:F160" totalsRowShown="0" headerRowDxfId="167">
   <autoFilter ref="A157:F160" xr:uid="{0F1F4D22-D736-AE47-A5E1-B5F142D02E52}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{525EECB4-0784-8D48-B16D-C694E9D9F3B8}" name="#"/>
@@ -2824,30 +2947,30 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{153F6715-F770-8740-94D2-11D1476495FA}" name="Table22" displayName="Table22" ref="A164:F166" totalsRowShown="0" headerRowDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{153F6715-F770-8740-94D2-11D1476495FA}" name="Table22" displayName="Table22" ref="A164:F166" totalsRowShown="0" headerRowDxfId="166">
   <autoFilter ref="A164:F166" xr:uid="{7B3DE3F3-BAF0-BF44-A7DA-9DFA68E3DC83}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D7DE3DBC-AAC4-484C-B044-C601FDAF02DC}" name="#"/>
-    <tableColumn id="2" xr3:uid="{C9A6B1AF-95A9-3645-91A9-222B0825EFB1}" name="KW" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{FB13CD5A-7791-E94E-BF99-B03DB836AA57}" name="VOLUME" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{7E5AC52B-EBF1-4E45-B5A4-45743185D627}" name="CPC" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{FA5B254D-C1A4-0740-928B-17E5D705D531}" name="PD" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{47C8AA8C-38E2-BB44-9527-FF94F70F2510}" name="SD" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{C9A6B1AF-95A9-3645-91A9-222B0825EFB1}" name="KW" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{FB13CD5A-7791-E94E-BF99-B03DB836AA57}" name="VOLUME" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{7E5AC52B-EBF1-4E45-B5A4-45743185D627}" name="CPC" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{FA5B254D-C1A4-0740-928B-17E5D705D531}" name="PD" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{47C8AA8C-38E2-BB44-9527-FF94F70F2510}" name="SD" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0782B336-FE7D-CC46-A30B-0629DECFFF6A}" name="Table23" displayName="Table23" ref="A169:F170" totalsRowShown="0" headerRowDxfId="150">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0782B336-FE7D-CC46-A30B-0629DECFFF6A}" name="Table23" displayName="Table23" ref="A169:F170" totalsRowShown="0" headerRowDxfId="165">
   <autoFilter ref="A169:F170" xr:uid="{97A80D7C-2CA8-8948-A0E2-772A6E732068}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2DE3AF2C-F140-7D4F-8B9F-EFA7A54EC4D0}" name="#"/>
-    <tableColumn id="2" xr3:uid="{46B29A82-2A3B-C04C-90EC-B4C152D77495}" name="KW" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{CD259F80-07DF-7F4A-9F6D-7347B1ABA398}" name="VOLUME" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{4D39A03D-9DE9-F343-AEFA-C8FC45D66B39}" name="CPC" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{906F2C6B-7E86-8E40-B607-0C6AAE941A07}" name="PD" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{0E1D0FA5-03CD-B04A-B657-31212FE5F18E}" name="SD" dataDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{46B29A82-2A3B-C04C-90EC-B4C152D77495}" name="KW" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{CD259F80-07DF-7F4A-9F6D-7347B1ABA398}" name="VOLUME" dataDxfId="133"/>
+    <tableColumn id="4" xr3:uid="{4D39A03D-9DE9-F343-AEFA-C8FC45D66B39}" name="CPC" dataDxfId="132"/>
+    <tableColumn id="5" xr3:uid="{906F2C6B-7E86-8E40-B607-0C6AAE941A07}" name="PD" dataDxfId="131"/>
+    <tableColumn id="6" xr3:uid="{0E1D0FA5-03CD-B04A-B657-31212FE5F18E}" name="SD" dataDxfId="130"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2873,11 +2996,11 @@
   <autoFilter ref="A180:F181" xr:uid="{8D239E99-0A9B-7940-BECF-DD4766F3562C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{679680AE-6A12-264D-93DA-A3C62351AF2E}" name="#"/>
-    <tableColumn id="2" xr3:uid="{4A761668-B2DA-4A48-80D3-9B51C3DB4E78}" name="KW"/>
-    <tableColumn id="3" xr3:uid="{704ECB16-EE1E-8741-98CB-56DB991AEDF9}" name="VOLUME"/>
-    <tableColumn id="4" xr3:uid="{CB97B695-C88B-A643-9C20-E7A08C061046}" name="CPC"/>
-    <tableColumn id="5" xr3:uid="{1AC47DCF-2E46-E246-B5F6-8E832020B408}" name="PD"/>
-    <tableColumn id="6" xr3:uid="{DEE67139-1D7E-4D4D-A805-7EE9A4ECCC68}" name="SD"/>
+    <tableColumn id="2" xr3:uid="{4A761668-B2DA-4A48-80D3-9B51C3DB4E78}" name="KW" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{704ECB16-EE1E-8741-98CB-56DB991AEDF9}" name="VOLUME" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{CB97B695-C88B-A643-9C20-E7A08C061046}" name="CPC" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{1AC47DCF-2E46-E246-B5F6-8E832020B408}" name="PD" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{DEE67139-1D7E-4D4D-A805-7EE9A4ECCC68}" name="SD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2888,11 +3011,11 @@
   <autoFilter ref="A184:F185" xr:uid="{B497B441-E5E6-EB44-8894-1324DA34F533}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D72FC37C-2105-8F4E-98EA-670BBF29CD17}" name="#"/>
-    <tableColumn id="2" xr3:uid="{5E44F6B5-6DF9-5146-AFAA-9C528D4D818D}" name="KW" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{C2FD83C0-C1F3-2949-98F0-E758CDB8BCBA}" name="VOLUME" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{7DA14CC2-991A-C145-B9EB-20DCC2423422}" name="CPC" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{650F3EB6-3A8C-ED47-BEF0-19DC9EE4C005}" name="PD" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{D7D380D4-CF29-C844-B40C-D5184EB459EF}" name="SD" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{5E44F6B5-6DF9-5146-AFAA-9C528D4D818D}" name="KW" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{C2FD83C0-C1F3-2949-98F0-E758CDB8BCBA}" name="VOLUME" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7DA14CC2-991A-C145-B9EB-20DCC2423422}" name="CPC" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{650F3EB6-3A8C-ED47-BEF0-19DC9EE4C005}" name="PD" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{D7D380D4-CF29-C844-B40C-D5184EB459EF}" name="SD" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2933,26 +3056,26 @@
   <autoFilter ref="A202:F204" xr:uid="{79FE5471-718D-D84D-B958-0F7ED66B7A62}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{FDF0208A-0A77-3C40-AF89-BDF5B12E55A8}" name="#"/>
-    <tableColumn id="2" xr3:uid="{E62E53B2-C6FA-F748-B88D-0682053BE258}" name="KW" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{C883B0A8-B5F8-4E40-B0F5-0561B644F681}" name="VOLUME" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{0F94DD56-CE6E-4040-BD92-64EC29767E07}" name="CPC" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{9E354F6A-FF22-3342-851E-32F99445E2BA}" name="PD" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{511904F2-7755-F943-8B73-B5D8997F0DF4}" name="SD" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{E62E53B2-C6FA-F748-B88D-0682053BE258}" name="KW" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{C883B0A8-B5F8-4E40-B0F5-0561B644F681}" name="VOLUME" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{0F94DD56-CE6E-4040-BD92-64EC29767E07}" name="CPC" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{9E354F6A-FF22-3342-851E-32F99445E2BA}" name="PD" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{511904F2-7755-F943-8B73-B5D8997F0DF4}" name="SD" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D27A6161-190E-6944-904F-43BED03777DD}" name="Table3" displayName="Table3" ref="A31:F39" totalsRowShown="0" headerRowDxfId="187" dataDxfId="188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D27A6161-190E-6944-904F-43BED03777DD}" name="Table3" displayName="Table3" ref="A31:F39" totalsRowShown="0" headerRowDxfId="202" dataDxfId="203">
   <autoFilter ref="A31:F39" xr:uid="{BDC9A2E4-574E-EC49-8529-7DB31751E3EA}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{09EE696F-DB41-2F48-A130-CE27A90F559F}" name="#"/>
     <tableColumn id="2" xr3:uid="{269AD9DE-D8B1-8045-8983-168EA7049F62}" name="KW"/>
-    <tableColumn id="3" xr3:uid="{F7C59FC9-DF64-FD40-8D2F-EF32939002B1}" name="VOLUME" dataDxfId="192"/>
-    <tableColumn id="4" xr3:uid="{7D2664FE-FC8A-9748-81FA-CCE7A833F5C7}" name="CPC" dataDxfId="191"/>
-    <tableColumn id="5" xr3:uid="{E5657E44-87CE-4E4C-8086-7953652A722B}" name="PD" dataDxfId="190"/>
-    <tableColumn id="6" xr3:uid="{661FCF7E-DA3E-514D-8DC7-7D06C45AACFC}" name="SD" dataDxfId="189"/>
+    <tableColumn id="3" xr3:uid="{F7C59FC9-DF64-FD40-8D2F-EF32939002B1}" name="VOLUME" dataDxfId="207"/>
+    <tableColumn id="4" xr3:uid="{7D2664FE-FC8A-9748-81FA-CCE7A833F5C7}" name="CPC" dataDxfId="206"/>
+    <tableColumn id="5" xr3:uid="{E5657E44-87CE-4E4C-8086-7953652A722B}" name="PD" dataDxfId="205"/>
+    <tableColumn id="6" xr3:uid="{661FCF7E-DA3E-514D-8DC7-7D06C45AACFC}" name="SD" dataDxfId="204"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3023,11 +3146,11 @@
   <autoFilter ref="A232:F233" xr:uid="{798DAC0A-477C-AE4E-A31E-727E21B359A3}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1A68CF93-2105-E843-9086-FF696EBEF9EB}" name="#"/>
-    <tableColumn id="2" xr3:uid="{10A455A8-44CC-1D40-B80E-88EA3F8674CD}" name="KW" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{ED2B36EA-BD98-2E4C-81A5-4FCDFFE06961}" name="VOLUME" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{A1D86550-0EC1-A348-A6A7-DE63593FD1DA}" name="CPC" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{1AB74525-825E-2747-A048-018E76DADD88}" name="PD" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{BC7C9624-2B36-5546-9348-F627A4622F57}" name="SD" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{10A455A8-44CC-1D40-B80E-88EA3F8674CD}" name="KW" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{ED2B36EA-BD98-2E4C-81A5-4FCDFFE06961}" name="VOLUME" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{A1D86550-0EC1-A348-A6A7-DE63593FD1DA}" name="CPC" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{1AB74525-825E-2747-A048-018E76DADD88}" name="PD" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{BC7C9624-2B36-5546-9348-F627A4622F57}" name="SD" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3038,11 +3161,11 @@
   <autoFilter ref="A236:F237" xr:uid="{4A881D36-4749-F74C-B36A-481354247021}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{FBAC947B-E7DF-9E45-B1A9-997D3AC3DDEB}" name="#"/>
-    <tableColumn id="2" xr3:uid="{8DB65BBD-94EE-B44E-938D-EB91731083D6}" name="KW" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{2571BFAF-55C8-8340-BFB8-04046ADBD13D}" name="VOLUME" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{2910A3E4-1B94-3A42-95DD-24B163F5F4C4}" name="CPC" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{278A0A9D-2373-D747-8565-D4AAB9FFB722}" name="PD" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{C9E1AE8B-F6FC-E94C-AEB4-B790F7139A14}" name="SD" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{8DB65BBD-94EE-B44E-938D-EB91731083D6}" name="KW" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{2571BFAF-55C8-8340-BFB8-04046ADBD13D}" name="VOLUME" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{2910A3E4-1B94-3A42-95DD-24B163F5F4C4}" name="CPC" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{278A0A9D-2373-D747-8565-D4AAB9FFB722}" name="PD" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{C9E1AE8B-F6FC-E94C-AEB4-B790F7139A14}" name="SD" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3053,11 +3176,11 @@
   <autoFilter ref="A241:F242" xr:uid="{C6A34C7A-FF1B-564F-9487-1F6564C55FB0}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{21007F4A-8E39-0A45-A357-7C287AB1B6A8}" name="#"/>
-    <tableColumn id="2" xr3:uid="{522AF2E7-8DD6-9A40-9946-E337745086F9}" name="KW" dataDxfId="129"/>
-    <tableColumn id="3" xr3:uid="{8A5E3EC2-0B37-B84D-85B5-8C66AED77238}" name="VOLUME" dataDxfId="128"/>
-    <tableColumn id="4" xr3:uid="{8DEF61B7-2DA8-1043-9E62-21687C2B9C0E}" name="CPC" dataDxfId="127"/>
-    <tableColumn id="5" xr3:uid="{154F65F6-6C82-6D43-B15B-1140E4CA3B47}" name="PD" dataDxfId="126"/>
-    <tableColumn id="6" xr3:uid="{7D2BA681-048E-FC4B-9F73-130EF4415D12}" name="SD" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{522AF2E7-8DD6-9A40-9946-E337745086F9}" name="KW" dataDxfId="144"/>
+    <tableColumn id="3" xr3:uid="{8A5E3EC2-0B37-B84D-85B5-8C66AED77238}" name="VOLUME" dataDxfId="143"/>
+    <tableColumn id="4" xr3:uid="{8DEF61B7-2DA8-1043-9E62-21687C2B9C0E}" name="CPC" dataDxfId="142"/>
+    <tableColumn id="5" xr3:uid="{154F65F6-6C82-6D43-B15B-1140E4CA3B47}" name="PD" dataDxfId="141"/>
+    <tableColumn id="6" xr3:uid="{7D2BA681-048E-FC4B-9F73-130EF4415D12}" name="SD" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3068,11 +3191,11 @@
   <autoFilter ref="A313:F315" xr:uid="{80917D28-E05D-744F-9B91-CFD6B0CB3F86}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3673096A-10E6-D84E-8AA4-8A832614FE9C}" name="#"/>
-    <tableColumn id="2" xr3:uid="{97C26049-DE12-1347-B001-DDA8A703812A}" name="KW" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{A1221B1E-A972-3143-9AF5-035B25146878}" name="VOLUME" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{886918F8-80E2-3143-81B7-26673EEE2732}" name="CPC" dataDxfId="147"/>
-    <tableColumn id="5" xr3:uid="{7138E072-4D42-AD49-9575-97359C1D6762}" name="PD" dataDxfId="146"/>
-    <tableColumn id="6" xr3:uid="{67A37A69-D6B6-FE45-B9BC-AE71C5D4192D}" name="SD" dataDxfId="145"/>
+    <tableColumn id="2" xr3:uid="{97C26049-DE12-1347-B001-DDA8A703812A}" name="KW" dataDxfId="164"/>
+    <tableColumn id="3" xr3:uid="{A1221B1E-A972-3143-9AF5-035B25146878}" name="VOLUME" dataDxfId="163"/>
+    <tableColumn id="4" xr3:uid="{886918F8-80E2-3143-81B7-26673EEE2732}" name="CPC" dataDxfId="162"/>
+    <tableColumn id="5" xr3:uid="{7138E072-4D42-AD49-9575-97359C1D6762}" name="PD" dataDxfId="161"/>
+    <tableColumn id="6" xr3:uid="{67A37A69-D6B6-FE45-B9BC-AE71C5D4192D}" name="SD" dataDxfId="160"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3109,15 +3232,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6CD6A3DA-EBB3-4B49-A333-F222C71C3FF4}" name="Table4" displayName="Table4" ref="A43:F50" totalsRowShown="0" headerRowDxfId="181" dataDxfId="182">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6CD6A3DA-EBB3-4B49-A333-F222C71C3FF4}" name="Table4" displayName="Table4" ref="A43:F50" totalsRowShown="0" headerRowDxfId="196" dataDxfId="197">
   <autoFilter ref="A43:F50" xr:uid="{E1F4886C-A78A-534F-9D7B-151A99238035}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5C5A6511-87CA-6640-8AF2-E538935E19D4}" name="#"/>
     <tableColumn id="2" xr3:uid="{AF38B8D5-D486-D44B-97B3-C65E46F807D2}" name="KW"/>
-    <tableColumn id="3" xr3:uid="{E06AF93F-99E3-8D4A-A8F6-8379012349BD}" name="VOLUME" dataDxfId="186"/>
-    <tableColumn id="4" xr3:uid="{B31113DE-7E56-DB4E-99BE-2FC580590D64}" name="CPC" dataDxfId="185"/>
-    <tableColumn id="5" xr3:uid="{3909BDF8-8D1B-C040-BEAA-7F91A66F34F4}" name="PD" dataDxfId="184"/>
-    <tableColumn id="6" xr3:uid="{F63EF63C-5693-7F40-A3E6-3D3B30C29EBE}" name="SD" dataDxfId="183"/>
+    <tableColumn id="3" xr3:uid="{E06AF93F-99E3-8D4A-A8F6-8379012349BD}" name="VOLUME" dataDxfId="201"/>
+    <tableColumn id="4" xr3:uid="{B31113DE-7E56-DB4E-99BE-2FC580590D64}" name="CPC" dataDxfId="200"/>
+    <tableColumn id="5" xr3:uid="{3909BDF8-8D1B-C040-BEAA-7F91A66F34F4}" name="PD" dataDxfId="199"/>
+    <tableColumn id="6" xr3:uid="{F63EF63C-5693-7F40-A3E6-3D3B30C29EBE}" name="SD" dataDxfId="198"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3128,11 +3251,11 @@
   <autoFilter ref="A297:F298" xr:uid="{8415CD92-C684-BD4D-BF4A-B93A3D7447AF}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{AA071852-22B1-B54C-B1F0-945B2C6D3A61}" name="#"/>
-    <tableColumn id="2" xr3:uid="{29452E80-0BC1-8346-8BE0-61AA79C4B88A}" name="KW" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{52CB9019-B229-EF45-BC98-375AAEC2014A}" name="VOLUME" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{93812977-0181-0244-A57F-EFC6BC94F412}" name="CPC" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{5C50DD7D-751A-9C4B-A697-2B64A55B5710}" name="PD" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{435C4AFB-34B3-7E49-8A55-5C2678C923C6}" name="SD" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{29452E80-0BC1-8346-8BE0-61AA79C4B88A}" name="KW" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{52CB9019-B229-EF45-BC98-375AAEC2014A}" name="VOLUME" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{93812977-0181-0244-A57F-EFC6BC94F412}" name="CPC" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{5C50DD7D-751A-9C4B-A697-2B64A55B5710}" name="PD" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{435C4AFB-34B3-7E49-8A55-5C2678C923C6}" name="SD" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3143,11 +3266,11 @@
   <autoFilter ref="A290:F292" xr:uid="{21312958-A3D9-5342-B8CD-58201E27E1AE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4E0F92E9-9CE0-7045-92BD-799AB5D715C8}" name="#"/>
-    <tableColumn id="2" xr3:uid="{311BB895-1944-E846-A97B-47A473B4B203}" name="KW" dataDxfId="134"/>
-    <tableColumn id="3" xr3:uid="{B8A9F904-9AAC-A04B-BF25-0D07CE4DF9B5}" name="VOLUME" dataDxfId="133"/>
-    <tableColumn id="4" xr3:uid="{D53E6C78-6A76-684F-BF86-0E32818949C2}" name="CPC" dataDxfId="132"/>
-    <tableColumn id="5" xr3:uid="{C7450CE3-EFFB-674D-A49F-5BB2801F623A}" name="PD" dataDxfId="131"/>
-    <tableColumn id="6" xr3:uid="{BE80AA8B-61FD-4946-88DC-3AA8B8A5FB25}" name="SD" dataDxfId="130"/>
+    <tableColumn id="2" xr3:uid="{311BB895-1944-E846-A97B-47A473B4B203}" name="KW" dataDxfId="149"/>
+    <tableColumn id="3" xr3:uid="{B8A9F904-9AAC-A04B-BF25-0D07CE4DF9B5}" name="VOLUME" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{D53E6C78-6A76-684F-BF86-0E32818949C2}" name="CPC" dataDxfId="147"/>
+    <tableColumn id="5" xr3:uid="{C7450CE3-EFFB-674D-A49F-5BB2801F623A}" name="PD" dataDxfId="146"/>
+    <tableColumn id="6" xr3:uid="{BE80AA8B-61FD-4946-88DC-3AA8B8A5FB25}" name="SD" dataDxfId="145"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3173,11 +3296,11 @@
   <autoFilter ref="A275:F276" xr:uid="{131C604D-C75F-6543-9E00-321A2AB0FC66}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{47479908-2CEB-F542-9F66-BF791B058A2B}" name="#"/>
-    <tableColumn id="2" xr3:uid="{7458C2FE-6FD9-9E4D-8864-B42898EA1C2D}" name="KW" dataDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{90BD3323-0AA7-7042-A506-170EC757793A}" name="VOLUME" dataDxfId="123"/>
-    <tableColumn id="4" xr3:uid="{1DBE8357-B843-1442-88B7-2E4685D34888}" name="CPC" dataDxfId="122"/>
-    <tableColumn id="5" xr3:uid="{D281F16B-9497-0A42-AFE9-23B682876E91}" name="PD" dataDxfId="121"/>
-    <tableColumn id="6" xr3:uid="{C599C896-EAED-DB4A-8987-F459D26B76EA}" name="SD" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{7458C2FE-6FD9-9E4D-8864-B42898EA1C2D}" name="KW" dataDxfId="139"/>
+    <tableColumn id="3" xr3:uid="{90BD3323-0AA7-7042-A506-170EC757793A}" name="VOLUME" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{1DBE8357-B843-1442-88B7-2E4685D34888}" name="CPC" dataDxfId="137"/>
+    <tableColumn id="5" xr3:uid="{D281F16B-9497-0A42-AFE9-23B682876E91}" name="PD" dataDxfId="136"/>
+    <tableColumn id="6" xr3:uid="{C599C896-EAED-DB4A-8987-F459D26B76EA}" name="SD" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3218,11 +3341,11 @@
   <autoFilter ref="A256:F258" xr:uid="{014F1DDF-A660-394F-A183-1D5B6B900C85}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{53E124B0-4460-2B4D-8288-EC3202FA39CC}" name="#"/>
-    <tableColumn id="2" xr3:uid="{49A67E34-5D4A-A24A-9E49-67B344A4D04A}" name="KW"/>
-    <tableColumn id="3" xr3:uid="{7439E611-39DD-AA4E-B590-466EA417795F}" name="VOLUME"/>
-    <tableColumn id="4" xr3:uid="{3E7DF6F4-1D73-BE4F-8FB1-433F9B3D46C0}" name="CPC"/>
-    <tableColumn id="5" xr3:uid="{D951D2E1-8503-5845-8723-DA1EC1038910}" name="PD"/>
-    <tableColumn id="6" xr3:uid="{66E2FF7E-44F5-8943-9487-8F706A046256}" name="SD"/>
+    <tableColumn id="2" xr3:uid="{49A67E34-5D4A-A24A-9E49-67B344A4D04A}" name="KW" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{7439E611-39DD-AA4E-B590-466EA417795F}" name="VOLUME" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{3E7DF6F4-1D73-BE4F-8FB1-433F9B3D46C0}" name="CPC" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{D951D2E1-8503-5845-8723-DA1EC1038910}" name="PD" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{66E2FF7E-44F5-8943-9487-8F706A046256}" name="SD" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3233,11 +3356,11 @@
   <autoFilter ref="A251:F252" xr:uid="{2605DB0E-565A-764E-B08C-2A49ABFBCFEB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{90201E4E-36D1-0B44-BA47-AE1B928B789B}" name="#"/>
-    <tableColumn id="2" xr3:uid="{5CF3D89A-BD7E-DF47-9AE5-54204B9DD67D}" name="KW" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{DB9E152C-CC10-D041-9FB7-DED0E4DD6F2F}" name="VOLUME" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{2129E822-B724-164C-AC71-6DF4EDA43B5E}" name="CPC" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{B487EB01-4CA2-AF46-8ABE-D5082F64B50F}" name="PD" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{615DA23E-F319-C546-BD1A-B626825BF969}" name="SD" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{5CF3D89A-BD7E-DF47-9AE5-54204B9DD67D}" name="KW" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{DB9E152C-CC10-D041-9FB7-DED0E4DD6F2F}" name="VOLUME" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{2129E822-B724-164C-AC71-6DF4EDA43B5E}" name="CPC" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{B487EB01-4CA2-AF46-8ABE-D5082F64B50F}" name="PD" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{615DA23E-F319-C546-BD1A-B626825BF969}" name="SD" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3274,15 +3397,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ABB0287C-E77D-FB4A-B57C-1F015485ED9B}" name="Table5" displayName="Table5" ref="A53:F64" totalsRowShown="0" headerRowDxfId="179" dataDxfId="180">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ABB0287C-E77D-FB4A-B57C-1F015485ED9B}" name="Table5" displayName="Table5" ref="A53:F64" totalsRowShown="0" headerRowDxfId="194" dataDxfId="195">
   <autoFilter ref="A53:F64" xr:uid="{40D9031D-B8B8-2649-9744-638C0B6C1119}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2445B845-753F-434D-994F-9611BF1B1819}" name="#"/>
-    <tableColumn id="2" xr3:uid="{A56AFC12-695B-3D48-AE65-A6A2003BA328}" name="KW" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{3C617472-002E-B649-8B2F-D9EBD0F31B9B}" name="VOLUME" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{7A7CB667-328D-C74B-A491-018716AAB431}" name="CPC" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{72F17B20-E61A-4E46-AFCC-F27E21C38A34}" name="PD" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{39A6763D-2427-4047-8F00-4EE6481B6817}" name="SD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{A56AFC12-695B-3D48-AE65-A6A2003BA328}" name="KW" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{3C617472-002E-B649-8B2F-D9EBD0F31B9B}" name="VOLUME" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{7A7CB667-328D-C74B-A491-018716AAB431}" name="CPC" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{72F17B20-E61A-4E46-AFCC-F27E21C38A34}" name="PD" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{39A6763D-2427-4047-8F00-4EE6481B6817}" name="SD" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3323,11 +3446,11 @@
   <autoFilter ref="A356:F358" xr:uid="{E616B480-8E79-C14D-85B9-E21CB859CEAD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{46FB6008-307F-894B-AF2B-7335CD5EF175}" name="#"/>
-    <tableColumn id="2" xr3:uid="{08D78948-637B-964C-AC65-A587329B555A}" name="KW" dataDxfId="144"/>
-    <tableColumn id="3" xr3:uid="{75E39E01-638B-8B41-B424-FEF42743F882}" name="VOLUME" dataDxfId="143"/>
-    <tableColumn id="4" xr3:uid="{A4499AF4-AC54-CA42-8A44-D3442A1E53CF}" name="CPC" dataDxfId="142"/>
-    <tableColumn id="5" xr3:uid="{C52B8664-213C-B34E-90E5-E0B9C24BDF6F}" name="PD" dataDxfId="141"/>
-    <tableColumn id="6" xr3:uid="{2A86F28E-29C5-B444-BC11-A45C0D4DB6C4}" name="SD" dataDxfId="140"/>
+    <tableColumn id="2" xr3:uid="{08D78948-637B-964C-AC65-A587329B555A}" name="KW" dataDxfId="159"/>
+    <tableColumn id="3" xr3:uid="{75E39E01-638B-8B41-B424-FEF42743F882}" name="VOLUME" dataDxfId="158"/>
+    <tableColumn id="4" xr3:uid="{A4499AF4-AC54-CA42-8A44-D3442A1E53CF}" name="CPC" dataDxfId="157"/>
+    <tableColumn id="5" xr3:uid="{C52B8664-213C-B34E-90E5-E0B9C24BDF6F}" name="PD" dataDxfId="156"/>
+    <tableColumn id="6" xr3:uid="{2A86F28E-29C5-B444-BC11-A45C0D4DB6C4}" name="SD" dataDxfId="155"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3338,11 +3461,11 @@
   <autoFilter ref="A361:F363" xr:uid="{C716696E-A16E-3F4B-9353-B6DE44744036}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4A5397EF-0CF6-E144-BA74-053A47927FEE}" name="#"/>
-    <tableColumn id="2" xr3:uid="{4B283485-6E41-B749-BF24-420220818E0E}" name="KW" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{2F7F200C-8B71-124F-8C4A-AFB9EA61FC34}" name="VOLUME" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{B39C4444-CE70-374A-A6B4-BB99F8B239BB}" name="CPC" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{3AF8CF54-3FA1-EE4F-A683-BF02D40C681B}" name="PD" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{C8E43254-08F1-4548-9DF5-24F730CD1DE4}" name="SD" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{4B283485-6E41-B749-BF24-420220818E0E}" name="KW" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{2F7F200C-8B71-124F-8C4A-AFB9EA61FC34}" name="VOLUME" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{B39C4444-CE70-374A-A6B4-BB99F8B239BB}" name="CPC" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{3AF8CF54-3FA1-EE4F-A683-BF02D40C681B}" name="PD" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{C8E43254-08F1-4548-9DF5-24F730CD1DE4}" name="SD" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3398,11 +3521,11 @@
   <autoFilter ref="A395:F396" xr:uid="{E1ABF0D9-1B82-D245-AB49-B1E6E7C794DD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5AD74509-C6BC-1040-A108-BF0B1E6DEB87}" name="#"/>
-    <tableColumn id="2" xr3:uid="{24E9E449-C266-5941-8312-29B99050AC2A}" name="KW" dataDxfId="139"/>
-    <tableColumn id="3" xr3:uid="{8E815F5F-D516-6B42-8054-E558941EB56B}" name="VOLUME" dataDxfId="138"/>
-    <tableColumn id="4" xr3:uid="{2EAE2FA4-58F0-4449-9BF9-2D55992E0A31}" name="CPC" dataDxfId="137"/>
-    <tableColumn id="5" xr3:uid="{99BCB5E3-2257-F344-A57E-65B9DBACCB15}" name="PD" dataDxfId="136"/>
-    <tableColumn id="6" xr3:uid="{51DC1A12-5999-0F43-98B0-EBF8E297BC80}" name="SD" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{24E9E449-C266-5941-8312-29B99050AC2A}" name="KW" dataDxfId="154"/>
+    <tableColumn id="3" xr3:uid="{8E815F5F-D516-6B42-8054-E558941EB56B}" name="VOLUME" dataDxfId="153"/>
+    <tableColumn id="4" xr3:uid="{2EAE2FA4-58F0-4449-9BF9-2D55992E0A31}" name="CPC" dataDxfId="152"/>
+    <tableColumn id="5" xr3:uid="{99BCB5E3-2257-F344-A57E-65B9DBACCB15}" name="PD" dataDxfId="151"/>
+    <tableColumn id="6" xr3:uid="{51DC1A12-5999-0F43-98B0-EBF8E297BC80}" name="SD" dataDxfId="150"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3413,71 +3536,71 @@
   <autoFilter ref="A399:F400" xr:uid="{258302AC-F1DF-CA48-887A-45506D3B0938}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{573199EB-F122-E54E-B615-7F620A4E0947}" name="#"/>
-    <tableColumn id="2" xr3:uid="{B215C889-9AA0-BC41-8B86-CC5233E98491}" name="KW" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{5FBA2203-B030-0A42-9A46-65E7F2D457EC}" name="VOLUME" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{6DC0A2F3-850B-F645-B4E0-BBEF8ECB2991}" name="CPC" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{AC957D1B-7210-5140-8CED-3FE636E39E39}" name="PD" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{4D603F8A-49D0-D445-A34A-8493CD1D0125}" name="SD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B215C889-9AA0-BC41-8B86-CC5233E98491}" name="KW" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{5FBA2203-B030-0A42-9A46-65E7F2D457EC}" name="VOLUME" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{6DC0A2F3-850B-F645-B4E0-BBEF8ECB2991}" name="CPC" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{AC957D1B-7210-5140-8CED-3FE636E39E39}" name="PD" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{4D603F8A-49D0-D445-A34A-8493CD1D0125}" name="SD" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{02D23F88-327F-BE42-8257-6FD3391D656B}" name="Table6" displayName="Table6" ref="A67:F76" totalsRowShown="0" headerRowDxfId="173" dataDxfId="174">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{02D23F88-327F-BE42-8257-6FD3391D656B}" name="Table6" displayName="Table6" ref="A67:F76" totalsRowShown="0" headerRowDxfId="188" dataDxfId="189">
   <autoFilter ref="A67:F76" xr:uid="{BC7DFAB6-8BA6-704C-B790-23A3C4748E5F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{880CBFAA-36A2-874D-8AA4-C09FE696FF00}" name="#"/>
     <tableColumn id="2" xr3:uid="{490F995D-E92F-964E-A5B6-8BAA9499424C}" name="KW"/>
-    <tableColumn id="3" xr3:uid="{6FFAB101-9047-FF46-934B-398B65EB3E43}" name="VOLUME" dataDxfId="178"/>
-    <tableColumn id="4" xr3:uid="{D00EF6C7-8B93-CD44-8985-FEB8E138E3F2}" name="CPC" dataDxfId="177"/>
-    <tableColumn id="5" xr3:uid="{94C4271F-E3BE-BD42-B077-4D1D09914322}" name="PD" dataDxfId="176"/>
-    <tableColumn id="6" xr3:uid="{047B9427-23EA-4D48-A22E-B0E6DA1C4F22}" name="SD" dataDxfId="175"/>
+    <tableColumn id="3" xr3:uid="{6FFAB101-9047-FF46-934B-398B65EB3E43}" name="VOLUME" dataDxfId="193"/>
+    <tableColumn id="4" xr3:uid="{D00EF6C7-8B93-CD44-8985-FEB8E138E3F2}" name="CPC" dataDxfId="192"/>
+    <tableColumn id="5" xr3:uid="{94C4271F-E3BE-BD42-B077-4D1D09914322}" name="PD" dataDxfId="191"/>
+    <tableColumn id="6" xr3:uid="{047B9427-23EA-4D48-A22E-B0E6DA1C4F22}" name="SD" dataDxfId="190"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{53E7CD98-E878-1B40-8A7D-834CDEA5211C}" name="Table7" displayName="Table7" ref="A79:F81" totalsRowShown="0" headerRowDxfId="171" dataDxfId="172">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{53E7CD98-E878-1B40-8A7D-834CDEA5211C}" name="Table7" displayName="Table7" ref="A79:F81" totalsRowShown="0" headerRowDxfId="186" dataDxfId="187">
   <autoFilter ref="A79:F81" xr:uid="{2CD78512-5E22-0B4A-8BE8-F391F61348D6}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9B309D2C-ED15-0547-B71A-7395F0F8857A}" name="#"/>
-    <tableColumn id="2" xr3:uid="{894DF4D9-C9E8-AB47-8B7C-BB2F4497A10A}" name="KW" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{54C9E742-B22C-E74E-85A4-6B6C26C8EEDA}" name="VOLUME" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{71C95C8A-91D3-3545-86F4-EC48906F2757}" name="CPC" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{EED0FBFF-0F6D-5642-9CF6-4054D7D47EDF}" name="PD" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{E85B43F9-EC9D-1445-8B45-9031F45AB06E}" name="SD" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{894DF4D9-C9E8-AB47-8B7C-BB2F4497A10A}" name="KW" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{54C9E742-B22C-E74E-85A4-6B6C26C8EEDA}" name="VOLUME" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{71C95C8A-91D3-3545-86F4-EC48906F2757}" name="CPC" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{EED0FBFF-0F6D-5642-9CF6-4054D7D47EDF}" name="PD" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{E85B43F9-EC9D-1445-8B45-9031F45AB06E}" name="SD" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{36461A84-FB1A-0540-9112-4CD67EA72ADF}" name="Table8" displayName="Table8" ref="A84:F90" totalsRowShown="0" headerRowDxfId="165" dataDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{36461A84-FB1A-0540-9112-4CD67EA72ADF}" name="Table8" displayName="Table8" ref="A84:F90" totalsRowShown="0" headerRowDxfId="180" dataDxfId="181">
   <autoFilter ref="A84:F90" xr:uid="{69D2BCC8-0473-C740-BF25-47E773E18FD8}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C673C655-553C-7240-821B-75AE6D0932DA}" name="#"/>
     <tableColumn id="2" xr3:uid="{E71D5422-955C-364E-A864-4CD804F9AF51}" name="KW"/>
-    <tableColumn id="3" xr3:uid="{6FDB4FD1-A82F-EE43-B6A9-34DB41DE2B43}" name="VOLUME" dataDxfId="170"/>
-    <tableColumn id="4" xr3:uid="{2C77C2F3-9602-C84E-9C3F-DE0D7F663514}" name="CPC" dataDxfId="169"/>
-    <tableColumn id="5" xr3:uid="{47D00704-BE8F-4440-BF1D-49398F51C47B}" name="PD" dataDxfId="168"/>
-    <tableColumn id="6" xr3:uid="{568B9501-3C39-4D49-AE83-5463E5AA43F9}" name="SD" dataDxfId="167"/>
+    <tableColumn id="3" xr3:uid="{6FDB4FD1-A82F-EE43-B6A9-34DB41DE2B43}" name="VOLUME" dataDxfId="185"/>
+    <tableColumn id="4" xr3:uid="{2C77C2F3-9602-C84E-9C3F-DE0D7F663514}" name="CPC" dataDxfId="184"/>
+    <tableColumn id="5" xr3:uid="{47D00704-BE8F-4440-BF1D-49398F51C47B}" name="PD" dataDxfId="183"/>
+    <tableColumn id="6" xr3:uid="{568B9501-3C39-4D49-AE83-5463E5AA43F9}" name="SD" dataDxfId="182"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2177E182-69D1-FB47-9F61-5EEEF5009111}" name="Table9" displayName="Table9" ref="A93:F95" totalsRowShown="0" headerRowDxfId="164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2177E182-69D1-FB47-9F61-5EEEF5009111}" name="Table9" displayName="Table9" ref="A93:F95" totalsRowShown="0" headerRowDxfId="179">
   <autoFilter ref="A93:F95" xr:uid="{713105D6-C097-A540-96E2-74085C8D355C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{32A9904F-5DF1-D141-BFB2-961239EF0309}" name="#"/>
-    <tableColumn id="2" xr3:uid="{C2231F29-B1B8-0B4F-B4C6-B50671407CC2}" name="KW" dataDxfId="99"/>
-    <tableColumn id="3" xr3:uid="{F826761F-77B6-DF42-A635-F0AFBC0AAD5F}" name="VOLUME" dataDxfId="98"/>
-    <tableColumn id="4" xr3:uid="{3F2823FB-FA28-5E44-A2CD-8F2E82ABEC26}" name="CPC" dataDxfId="97"/>
-    <tableColumn id="5" xr3:uid="{AB2C69DF-3990-CE45-9D49-83E82C772525}" name="PD" dataDxfId="96"/>
-    <tableColumn id="6" xr3:uid="{116930A3-9A25-854A-AC6E-697E7BB1C743}" name="SD" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{C2231F29-B1B8-0B4F-B4C6-B50671407CC2}" name="KW" dataDxfId="114"/>
+    <tableColumn id="3" xr3:uid="{F826761F-77B6-DF42-A635-F0AFBC0AAD5F}" name="VOLUME" dataDxfId="113"/>
+    <tableColumn id="4" xr3:uid="{3F2823FB-FA28-5E44-A2CD-8F2E82ABEC26}" name="CPC" dataDxfId="112"/>
+    <tableColumn id="5" xr3:uid="{AB2C69DF-3990-CE45-9D49-83E82C772525}" name="PD" dataDxfId="111"/>
+    <tableColumn id="6" xr3:uid="{116930A3-9A25-854A-AC6E-697E7BB1C743}" name="SD" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3782,8 +3905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA13C51-9151-4F4E-9D73-B21191CD2586}">
   <dimension ref="A1:J400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80:F81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5925,19 +6048,19 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B148" t="s">
+      <c r="B148" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="4">
         <v>40</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E148">
+      <c r="E148" s="4">
         <v>5</v>
       </c>
-      <c r="F148">
+      <c r="F148" s="4">
         <v>15</v>
       </c>
     </row>
@@ -6019,36 +6142,36 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B158" t="s">
+      <c r="B158" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C158">
+      <c r="C158" s="4">
         <v>20</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E158">
+      <c r="E158" s="4">
         <v>18</v>
       </c>
-      <c r="F158">
+      <c r="F158" s="4">
         <v>19</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B159" t="s">
+      <c r="B159" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C159">
+      <c r="C159" s="4">
         <v>10</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D159" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E159">
+      <c r="E159" s="4">
         <v>15</v>
       </c>
-      <c r="F159">
+      <c r="F159" s="4">
         <v>18</v>
       </c>
     </row>
@@ -6301,19 +6424,19 @@
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B181" t="s">
+      <c r="B181" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="4">
         <v>50</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E181">
+      <c r="E181" s="4">
         <v>16</v>
       </c>
-      <c r="F181">
+      <c r="F181" s="4">
         <v>23</v>
       </c>
     </row>
@@ -6395,19 +6518,19 @@
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B190" t="s">
+      <c r="B190" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C190">
+      <c r="C190" s="4">
         <v>70</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E190">
+      <c r="E190" s="4">
         <v>91</v>
       </c>
-      <c r="F190">
+      <c r="F190" s="4">
         <v>33</v>
       </c>
     </row>
@@ -6445,24 +6568,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B193" t="s">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B193" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="C193">
+      <c r="C193" s="4">
         <v>10</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E193">
+      <c r="E193" s="4">
         <v>59</v>
       </c>
-      <c r="F193">
+      <c r="F193" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B194" s="4" t="s">
         <v>265</v>
       </c>
@@ -6479,7 +6602,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B195" s="4" t="s">
         <v>267</v>
       </c>
@@ -6496,7 +6619,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>159</v>
       </c>
@@ -6506,7 +6629,7 @@
       <c r="E197" s="2"/>
       <c r="F197" s="2"/>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>0</v>
       </c>
@@ -6526,7 +6649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>158</v>
       </c>
@@ -6542,8 +6665,14 @@
       <c r="F199">
         <v>44</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G199" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H199" s="2"/>
+      <c r="I199" s="2"/>
+      <c r="J199" s="2"/>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>162</v>
       </c>
@@ -6553,7 +6682,7 @@
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>0</v>
       </c>
@@ -6573,7 +6702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B203" s="4" t="s">
         <v>160</v>
       </c>
@@ -6590,7 +6719,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B204" s="4" t="s">
         <v>269</v>
       </c>
@@ -6607,7 +6736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>168</v>
       </c>
@@ -6617,7 +6746,7 @@
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>0</v>
       </c>
@@ -6637,7 +6766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B208" s="4" t="s">
         <v>164</v>
       </c>
@@ -6834,36 +6963,36 @@
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B223" t="s">
+      <c r="B223" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C223">
+      <c r="C223" s="4">
         <v>20</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D223" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E223">
+      <c r="E223" s="4">
         <v>53</v>
       </c>
-      <c r="F223">
+      <c r="F223" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B224" t="s">
+      <c r="B224" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C224">
+      <c r="C224" s="4">
         <v>20</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D224" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E224">
+      <c r="E224" s="4">
         <v>25</v>
       </c>
-      <c r="F224">
+      <c r="F224" s="4">
         <v>13</v>
       </c>
     </row>
@@ -7214,36 +7343,36 @@
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B257" t="s">
+      <c r="B257" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C257">
+      <c r="C257" s="4">
         <v>20</v>
       </c>
-      <c r="D257" t="s">
+      <c r="D257" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E257">
+      <c r="E257" s="4">
         <v>100</v>
       </c>
-      <c r="F257">
+      <c r="F257" s="4">
         <v>36</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B258" t="s">
+      <c r="B258" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C258">
+      <c r="C258" s="4">
         <v>10</v>
       </c>
-      <c r="D258" t="s">
+      <c r="D258" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E258">
+      <c r="E258" s="4">
         <v>94</v>
       </c>
-      <c r="F258">
+      <c r="F258" s="4">
         <v>47</v>
       </c>
     </row>
@@ -8589,19 +8718,19 @@
       </c>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B373" t="s">
+      <c r="B373" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C373">
+      <c r="C373" s="4">
         <v>10</v>
       </c>
-      <c r="D373" t="s">
+      <c r="D373" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E373">
+      <c r="E373" s="4">
         <v>57</v>
       </c>
-      <c r="F373">
+      <c r="F373" s="4">
         <v>23</v>
       </c>
     </row>
@@ -8699,36 +8828,36 @@
       </c>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B382" t="s">
+      <c r="B382" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="C382">
+      <c r="C382" s="4">
         <v>40</v>
       </c>
-      <c r="D382" t="s">
+      <c r="D382" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="E382">
+      <c r="E382" s="4">
         <v>7</v>
       </c>
-      <c r="F382">
+      <c r="F382" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B383" t="s">
+      <c r="B383" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="C383">
+      <c r="C383" s="4">
         <v>40</v>
       </c>
-      <c r="D383" t="s">
+      <c r="D383" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E383">
+      <c r="E383" s="4">
         <v>0</v>
       </c>
-      <c r="F383">
+      <c r="F383" s="4">
         <v>18</v>
       </c>
     </row>
@@ -8784,19 +8913,19 @@
       </c>
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B387" t="s">
+      <c r="B387" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="C387">
+      <c r="C387" s="4">
         <v>10</v>
       </c>
-      <c r="D387" t="s">
+      <c r="D387" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E387">
+      <c r="E387" s="4">
         <v>0</v>
       </c>
-      <c r="F387">
+      <c r="F387" s="4">
         <v>5</v>
       </c>
     </row>
@@ -8835,53 +8964,53 @@
       </c>
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B390" t="s">
+      <c r="B390" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="C390">
+      <c r="C390" s="4">
         <v>20</v>
       </c>
-      <c r="D390" t="s">
+      <c r="D390" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E390">
+      <c r="E390" s="4">
         <v>6</v>
       </c>
-      <c r="F390">
+      <c r="F390" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B391" t="s">
+      <c r="B391" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="C391">
+      <c r="C391" s="4">
         <v>30</v>
       </c>
-      <c r="D391" t="s">
+      <c r="D391" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E391">
+      <c r="E391" s="4">
         <v>27</v>
       </c>
-      <c r="F391">
+      <c r="F391" s="4">
         <v>26</v>
       </c>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B392" t="s">
+      <c r="B392" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="C392">
+      <c r="C392" s="4">
         <v>40</v>
       </c>
-      <c r="D392" t="s">
+      <c r="D392" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E392">
+      <c r="E392" s="4">
         <v>2</v>
       </c>
-      <c r="F392">
+      <c r="F392" s="4">
         <v>14</v>
       </c>
     </row>
@@ -8972,12 +9101,13 @@
       <c r="F400" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
     <mergeCell ref="B366:F366"/>
     <mergeCell ref="B375:F375"/>
     <mergeCell ref="A380:F380"/>
     <mergeCell ref="A394:F394"/>
     <mergeCell ref="A398:F398"/>
+    <mergeCell ref="G199:J199"/>
     <mergeCell ref="G59:J59"/>
     <mergeCell ref="A318:F318"/>
     <mergeCell ref="A330:F330"/>

</xml_diff>